<commit_message>
Firmware coding started. LCD and encoder running
todos
- encoder change from polling to interrupt usage
- switch input connected to interrupt input
</commit_message>
<xml_diff>
--- a/Documents/Port_Usage_Planning.xlsx
+++ b/Documents/Port_Usage_Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juerg\Documents\_Workspaces\SaunaControlUnit\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACEBD14-CB58-4988-B82B-97AA4D98A635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7DA0D4-81DE-4035-A1B5-50D86FA12D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ESP pin usage" sheetId="6" r:id="rId1"/>
@@ -406,9 +406,6 @@
     <t>ENC_CLK</t>
   </si>
   <si>
-    <t>GPI17</t>
-  </si>
-  <si>
     <t>ESP32 necessary signals</t>
   </si>
   <si>
@@ -442,6 +439,9 @@
   <si>
     <t>The pins D0, D1, D2, D3, CMD and CLK are used internally for communication between ESP32 and SPI flash memory. 
 They are grouped on both sides near the USB connector. Avoid using these pins, as it may disrupt access to the SPI flash memory/SPI RAM.</t>
+  </si>
+  <si>
+    <t>GPIO17</t>
   </si>
 </sst>
 </file>
@@ -775,18 +775,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -804,56 +792,68 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1391,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9221DBC-EDCA-460E-9237-EA76481AB5F0}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1409,22 +1409,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="H1" s="59" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="H1" s="36" t="s">
-        <v>131</v>
-      </c>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
@@ -1440,7 +1440,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F2" s="20" t="s">
         <v>19</v>
@@ -1464,10 +1464,10 @@
       <c r="A3" s="21">
         <v>1</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="51" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="3"/>
@@ -1478,10 +1478,10 @@
       <c r="H3" s="21">
         <v>1</v>
       </c>
-      <c r="I3" s="56" t="s">
+      <c r="I3" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="56" t="s">
+      <c r="J3" s="51" t="s">
         <v>50</v>
       </c>
       <c r="K3" s="3"/>
@@ -1494,10 +1494,10 @@
       <c r="A4" s="21">
         <v>2</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="51" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="3"/>
@@ -1508,10 +1508,10 @@
       <c r="H4" s="21">
         <v>2</v>
       </c>
-      <c r="I4" s="56" t="s">
+      <c r="I4" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="J4" s="56" t="s">
+      <c r="J4" s="51" t="s">
         <v>35</v>
       </c>
       <c r="K4" s="3"/>
@@ -1524,10 +1524,10 @@
       <c r="A5" s="23">
         <v>3</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="54" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1542,10 +1542,10 @@
       <c r="H5" s="34">
         <v>3</v>
       </c>
-      <c r="I5" s="57" t="s">
+      <c r="I5" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="J5" s="57" t="s">
+      <c r="J5" s="52" t="s">
         <v>35</v>
       </c>
       <c r="K5" s="16" t="s">
@@ -1562,10 +1562,10 @@
       <c r="A6" s="23">
         <v>4</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="54" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -1580,10 +1580,10 @@
       <c r="H6" s="21">
         <v>4</v>
       </c>
-      <c r="I6" s="56" t="s">
+      <c r="I6" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="J6" s="56" t="s">
+      <c r="J6" s="51" t="s">
         <v>35</v>
       </c>
       <c r="K6" s="3"/>
@@ -1596,10 +1596,10 @@
       <c r="A7" s="23">
         <v>5</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="54" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -1614,10 +1614,10 @@
       <c r="H7" s="21">
         <v>5</v>
       </c>
-      <c r="I7" s="56" t="s">
+      <c r="I7" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="56" t="s">
+      <c r="J7" s="51" t="s">
         <v>35</v>
       </c>
       <c r="K7" s="3"/>
@@ -1630,10 +1630,10 @@
       <c r="A8" s="23">
         <v>6</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="54" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -1648,10 +1648,10 @@
       <c r="H8" s="34">
         <v>6</v>
       </c>
-      <c r="I8" s="57" t="s">
+      <c r="I8" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="J8" s="57" t="s">
+      <c r="J8" s="52" t="s">
         <v>35</v>
       </c>
       <c r="K8" s="16" t="s">
@@ -1668,10 +1668,10 @@
       <c r="A9" s="25">
         <v>7</v>
       </c>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="C9" s="57" t="s">
         <v>35</v>
       </c>
       <c r="D9" s="9" t="s">
@@ -1686,10 +1686,10 @@
       <c r="H9" s="21">
         <v>7</v>
       </c>
-      <c r="I9" s="56" t="s">
+      <c r="I9" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="J9" s="56" t="s">
+      <c r="J9" s="51" t="s">
         <v>50</v>
       </c>
       <c r="K9" s="3"/>
@@ -1702,10 +1702,10 @@
       <c r="A10" s="25">
         <v>8</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="62" t="s">
+      <c r="C10" s="57" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="9" t="s">
@@ -1720,10 +1720,10 @@
       <c r="H10" s="27">
         <v>8</v>
       </c>
-      <c r="I10" s="58" t="s">
+      <c r="I10" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="J10" s="58" t="s">
+      <c r="J10" s="53" t="s">
         <v>35</v>
       </c>
       <c r="K10" s="11" t="s">
@@ -1740,10 +1740,10 @@
       <c r="A11" s="25">
         <v>9</v>
       </c>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="62" t="s">
+      <c r="C11" s="57" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="9" t="s">
@@ -1755,17 +1755,17 @@
       <c r="F11" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="48">
+      <c r="H11" s="43">
         <v>9</v>
       </c>
-      <c r="I11" s="52" t="s">
+      <c r="I11" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="J11" s="52" t="s">
+      <c r="J11" s="47" t="s">
         <v>35</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L11" s="9" t="s">
         <v>13</v>
@@ -1778,28 +1778,28 @@
       <c r="A12" s="27">
         <v>10</v>
       </c>
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="58" t="s">
+      <c r="C12" s="53" t="s">
         <v>35</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F12" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="48">
+      <c r="H12" s="43">
         <v>10</v>
       </c>
-      <c r="I12" s="52" t="s">
+      <c r="I12" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="J12" s="52" t="s">
+      <c r="J12" s="47" t="s">
         <v>35</v>
       </c>
       <c r="K12" s="9" t="s">
@@ -1816,28 +1816,28 @@
       <c r="A13" s="27">
         <v>11</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="58" t="s">
+      <c r="C13" s="53" t="s">
         <v>35</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F13" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="48">
+      <c r="H13" s="43">
         <v>11</v>
       </c>
-      <c r="I13" s="52" t="s">
+      <c r="I13" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="J13" s="52" t="s">
+      <c r="J13" s="47" t="s">
         <v>35</v>
       </c>
       <c r="K13" s="9" t="s">
@@ -1854,17 +1854,17 @@
       <c r="A14" s="27">
         <v>12</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="58" t="s">
+      <c r="C14" s="53" t="s">
         <v>35</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F14" s="28" t="s">
         <v>46</v>
@@ -1872,10 +1872,10 @@
       <c r="H14" s="21">
         <v>12</v>
       </c>
-      <c r="I14" s="56" t="s">
+      <c r="I14" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="J14" s="56" t="s">
+      <c r="J14" s="51" t="s">
         <v>35</v>
       </c>
       <c r="K14" s="3"/>
@@ -1888,10 +1888,10 @@
       <c r="A15" s="25">
         <v>13</v>
       </c>
-      <c r="B15" s="62" t="s">
+      <c r="B15" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="62" t="s">
+      <c r="C15" s="57" t="s">
         <v>35</v>
       </c>
       <c r="D15" s="9" t="s">
@@ -1906,14 +1906,14 @@
       <c r="H15" s="23">
         <v>13</v>
       </c>
-      <c r="I15" s="59" t="s">
+      <c r="I15" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="J15" s="59" t="s">
+      <c r="J15" s="54" t="s">
         <v>35</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L15" s="7" t="s">
         <v>12</v>
@@ -1926,10 +1926,10 @@
       <c r="A16" s="21">
         <v>14</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C16" s="51" t="s">
         <v>50</v>
       </c>
       <c r="D16" s="3"/>
@@ -1940,10 +1940,10 @@
       <c r="H16" s="21">
         <v>14</v>
       </c>
-      <c r="I16" s="56" t="s">
+      <c r="I16" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="J16" s="56" t="s">
+      <c r="J16" s="51" t="s">
         <v>35</v>
       </c>
       <c r="K16" s="3"/>
@@ -1956,10 +1956,10 @@
       <c r="A17" s="25">
         <v>15</v>
       </c>
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="62" t="s">
+      <c r="C17" s="57" t="s">
         <v>35</v>
       </c>
       <c r="D17" s="9" t="s">
@@ -1974,10 +1974,10 @@
       <c r="H17" s="21">
         <v>16</v>
       </c>
-      <c r="I17" s="56" t="s">
+      <c r="I17" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="J17" s="56" t="s">
+      <c r="J17" s="51" t="s">
         <v>35</v>
       </c>
       <c r="K17" s="3"/>
@@ -1987,27 +1987,27 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="40">
+      <c r="A18" s="36">
         <v>16</v>
       </c>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="60" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="42" t="s">
+      <c r="C18" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="H18" s="48">
+      <c r="H18" s="43">
         <v>17</v>
       </c>
-      <c r="I18" s="52" t="s">
+      <c r="I18" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="J18" s="52" t="s">
+      <c r="J18" s="47" t="s">
         <v>35</v>
       </c>
       <c r="K18" s="9" t="s">
@@ -2021,62 +2021,62 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="40">
+      <c r="A19" s="36">
         <v>17</v>
       </c>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="60" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="43" t="s">
+      <c r="C19" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="H19" s="40">
+      <c r="H19" s="36">
         <v>17</v>
       </c>
-      <c r="I19" s="60" t="s">
+      <c r="I19" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="J19" s="60" t="s">
-        <v>35</v>
-      </c>
-      <c r="K19" s="41"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="42" t="s">
+      <c r="J19" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="38" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="40">
+      <c r="A20" s="36">
         <v>18</v>
       </c>
-      <c r="B20" s="60" t="s">
+      <c r="B20" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="60" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="42" t="s">
+      <c r="C20" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="H20" s="40">
+      <c r="H20" s="36">
         <v>18</v>
       </c>
-      <c r="I20" s="60" t="s">
+      <c r="I20" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="J20" s="60" t="s">
-        <v>35</v>
-      </c>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="42" t="s">
+      <c r="J20" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="38" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2084,10 +2084,10 @@
       <c r="A21" s="31">
         <v>19</v>
       </c>
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="63" t="s">
+      <c r="C21" s="58" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="32"/>
@@ -2095,107 +2095,107 @@
       <c r="F21" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="H21" s="44">
+      <c r="H21" s="40">
         <v>19</v>
       </c>
-      <c r="I21" s="61" t="s">
+      <c r="I21" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="J21" s="61" t="s">
-        <v>35</v>
-      </c>
-      <c r="K21" s="45"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="46" t="s">
+      <c r="J21" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="K21" s="41"/>
+      <c r="L21" s="41"/>
+      <c r="M21" s="42" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="61" t="s">
         <v>116</v>
       </c>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="37"/>
-      <c r="M23" s="37"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="60"/>
+      <c r="M23" s="60"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="61" t="s">
         <v>117</v>
       </c>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="37"/>
-      <c r="L25" s="37"/>
-      <c r="M25" s="37"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="60"/>
+      <c r="L25" s="60"/>
+      <c r="M25" s="60"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="47" t="s">
-        <v>135</v>
-      </c>
-      <c r="B27" s="47"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="47"/>
-      <c r="J27" s="47"/>
-      <c r="K27" s="47"/>
-      <c r="L27" s="47"/>
-      <c r="M27" s="47"/>
+      <c r="A27" s="62" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" s="62"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="62"/>
+      <c r="K27" s="62"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="62"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="47"/>
-      <c r="B28" s="47"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="47"/>
-      <c r="L28" s="47"/>
-      <c r="M28" s="47"/>
+      <c r="A28" s="62"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="62"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="62"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="47"/>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="47"/>
-      <c r="M29" s="47"/>
+      <c r="A29" s="62"/>
+      <c r="B29" s="62"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="62"/>
+      <c r="K29" s="62"/>
+      <c r="L29" s="62"/>
+      <c r="M29" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2207,6 +2207,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A25" r:id="rId1" xr:uid="{8C29EB1E-5FC7-4B4B-B6D2-9EF086296AB7}"/>
+    <hyperlink ref="A23" r:id="rId2" xr:uid="{66CDB618-6607-4CC0-9408-30BF1EA62DE2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2216,8 +2217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2243,31 +2244,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
+      <c r="A1" s="63" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="O1" s="59" t="s">
         <v>130</v>
       </c>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="O1" s="36" t="s">
-        <v>131</v>
-      </c>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
     </row>
     <row r="2" spans="1:20" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
@@ -2282,10 +2283,10 @@
       <c r="D2" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="50" t="s">
-        <v>126</v>
-      </c>
-      <c r="F2" s="50" t="s">
+      <c r="E2" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" s="45" t="s">
         <v>100</v>
       </c>
       <c r="H2" s="18" t="s">
@@ -2301,7 +2302,7 @@
         <v>4</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M2" s="20" t="s">
         <v>19</v>
@@ -2335,10 +2336,10 @@
       <c r="D3" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E3" s="51">
+      <c r="E3" s="46">
         <v>1</v>
       </c>
-      <c r="F3" s="51">
+      <c r="F3" s="46">
         <v>3</v>
       </c>
       <c r="H3" s="21">
@@ -2384,10 +2385,10 @@
       <c r="D4" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E4" s="51">
+      <c r="E4" s="46">
         <v>1</v>
       </c>
-      <c r="F4" s="51">
+      <c r="F4" s="46">
         <v>4</v>
       </c>
       <c r="H4" s="21">
@@ -2433,10 +2434,10 @@
       <c r="D5" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E5" s="51">
+      <c r="E5" s="46">
         <v>1</v>
       </c>
-      <c r="F5" s="51">
+      <c r="F5" s="46">
         <v>5</v>
       </c>
       <c r="H5" s="23">
@@ -2486,10 +2487,10 @@
       <c r="D6" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E6" s="51">
+      <c r="E6" s="46">
         <v>1</v>
       </c>
-      <c r="F6" s="51">
+      <c r="F6" s="46">
         <v>6</v>
       </c>
       <c r="H6" s="23">
@@ -2575,10 +2576,10 @@
       <c r="D8" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E8" s="52">
+      <c r="E8" s="47">
         <v>1</v>
       </c>
-      <c r="F8" s="52">
+      <c r="F8" s="47">
         <v>7</v>
       </c>
       <c r="G8" s="17"/>
@@ -2629,10 +2630,10 @@
       <c r="D9" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E9" s="52">
+      <c r="E9" s="47">
         <v>1</v>
       </c>
-      <c r="F9" s="52">
+      <c r="F9" s="47">
         <v>8</v>
       </c>
       <c r="G9" s="17"/>
@@ -2683,10 +2684,10 @@
       <c r="D10" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E10" s="52">
+      <c r="E10" s="47">
         <v>1</v>
       </c>
-      <c r="F10" s="52">
+      <c r="F10" s="47">
         <v>9</v>
       </c>
       <c r="H10" s="25">
@@ -2728,8 +2729,8 @@
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
       <c r="G11" s="17"/>
       <c r="H11" s="25">
         <v>9</v>
@@ -2750,7 +2751,7 @@
         <v>40</v>
       </c>
       <c r="N11" s="6"/>
-      <c r="O11" s="48">
+      <c r="O11" s="43">
         <v>9</v>
       </c>
       <c r="P11" s="9" t="s">
@@ -2760,7 +2761,7 @@
         <v>35</v>
       </c>
       <c r="R11" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="S11" s="9" t="s">
         <v>13</v>
@@ -2782,10 +2783,10 @@
       <c r="D12" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E12" s="54">
+      <c r="E12" s="49">
         <v>1</v>
       </c>
-      <c r="F12" s="54">
+      <c r="F12" s="49">
         <v>10</v>
       </c>
       <c r="G12" s="17"/>
@@ -2808,7 +2809,7 @@
         <v>42</v>
       </c>
       <c r="N12" s="6"/>
-      <c r="O12" s="48">
+      <c r="O12" s="43">
         <v>10</v>
       </c>
       <c r="P12" s="9" t="s">
@@ -2840,10 +2841,10 @@
       <c r="D13" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E13" s="54">
+      <c r="E13" s="49">
         <v>1</v>
       </c>
-      <c r="F13" s="54">
+      <c r="F13" s="49">
         <v>11</v>
       </c>
       <c r="G13" s="17"/>
@@ -2866,7 +2867,7 @@
         <v>44</v>
       </c>
       <c r="N13" s="6"/>
-      <c r="O13" s="48">
+      <c r="O13" s="43">
         <v>11</v>
       </c>
       <c r="P13" s="9" t="s">
@@ -2898,10 +2899,10 @@
       <c r="D14" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="E14" s="54">
+      <c r="E14" s="49">
         <v>1</v>
       </c>
-      <c r="F14" s="54">
+      <c r="F14" s="49">
         <v>12</v>
       </c>
       <c r="H14" s="27">
@@ -2943,8 +2944,8 @@
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
       <c r="H15" s="25">
         <v>13</v>
       </c>
@@ -2974,7 +2975,7 @@
         <v>35</v>
       </c>
       <c r="R15" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S15" s="7" t="s">
         <v>12</v>
@@ -2996,10 +2997,10 @@
       <c r="D16" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="52">
+      <c r="E16" s="47">
         <v>1</v>
       </c>
-      <c r="F16" s="52">
+      <c r="F16" s="47">
         <v>13</v>
       </c>
       <c r="H16" s="21">
@@ -3045,10 +3046,10 @@
       <c r="D17" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E17" s="52">
+      <c r="E17" s="47">
         <v>1</v>
       </c>
-      <c r="F17" s="52">
+      <c r="F17" s="47">
         <v>15</v>
       </c>
       <c r="H17" s="25">
@@ -3096,29 +3097,29 @@
         <v>15</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E18" s="52">
+        <v>128</v>
+      </c>
+      <c r="E18" s="47">
         <v>2</v>
       </c>
-      <c r="F18" s="52">
+      <c r="F18" s="47">
         <v>17</v>
       </c>
-      <c r="H18" s="40">
+      <c r="H18" s="36">
         <v>16</v>
       </c>
-      <c r="I18" s="41" t="s">
+      <c r="I18" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="J18" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="42" t="s">
+      <c r="J18" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="O18" s="48">
+      <c r="O18" s="43">
         <v>17</v>
       </c>
       <c r="P18" s="9" t="s">
@@ -3142,34 +3143,34 @@
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="H19" s="40">
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="H19" s="36">
         <v>17</v>
       </c>
-      <c r="I19" s="41" t="s">
+      <c r="I19" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="J19" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="K19" s="41"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="43" t="s">
+      <c r="J19" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="O19" s="40">
+      <c r="O19" s="36">
         <v>17</v>
       </c>
-      <c r="P19" s="41" t="s">
+      <c r="P19" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="Q19" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="R19" s="41"/>
-      <c r="S19" s="41"/>
-      <c r="T19" s="42" t="s">
+      <c r="Q19" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="R19" s="37"/>
+      <c r="S19" s="37"/>
+      <c r="T19" s="38" t="s">
         <v>90</v>
       </c>
     </row>
@@ -3186,38 +3187,38 @@
       <c r="D20" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="E20" s="55">
+      <c r="E20" s="50">
         <v>2</v>
       </c>
-      <c r="F20" s="55">
+      <c r="F20" s="50">
         <v>3</v>
       </c>
-      <c r="H20" s="40">
+      <c r="H20" s="36">
         <v>18</v>
       </c>
-      <c r="I20" s="41" t="s">
+      <c r="I20" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="J20" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="42" t="s">
+      <c r="J20" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="O20" s="40">
+      <c r="O20" s="36">
         <v>18</v>
       </c>
-      <c r="P20" s="41" t="s">
+      <c r="P20" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="Q20" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="R20" s="41"/>
-      <c r="S20" s="41"/>
-      <c r="T20" s="42" t="s">
+      <c r="Q20" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="R20" s="37"/>
+      <c r="S20" s="37"/>
+      <c r="T20" s="38" t="s">
         <v>92</v>
       </c>
     </row>
@@ -3234,10 +3235,10 @@
       <c r="D21" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="E21" s="55">
+      <c r="E21" s="50">
         <v>2</v>
       </c>
-      <c r="F21" s="55">
+      <c r="F21" s="50">
         <v>6</v>
       </c>
       <c r="H21" s="31">
@@ -3255,18 +3256,18 @@
         <v>61</v>
       </c>
       <c r="N21" s="6"/>
-      <c r="O21" s="44">
+      <c r="O21" s="40">
         <v>19</v>
       </c>
-      <c r="P21" s="45" t="s">
+      <c r="P21" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="Q21" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="R21" s="45"/>
-      <c r="S21" s="45"/>
-      <c r="T21" s="46" t="s">
+      <c r="Q21" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="R21" s="41"/>
+      <c r="S21" s="41"/>
+      <c r="T21" s="42" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3283,10 +3284,10 @@
       <c r="D22" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E22" s="54">
+      <c r="E22" s="49">
         <v>2</v>
       </c>
-      <c r="F22" s="54">
+      <c r="F22" s="49">
         <v>8</v>
       </c>
     </row>
@@ -3295,21 +3296,21 @@
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="49"/>
-      <c r="N23" s="49"/>
-      <c r="O23" s="49"/>
-      <c r="P23" s="49"/>
-      <c r="Q23" s="49"/>
-      <c r="R23" s="49"/>
-      <c r="S23" s="49"/>
-      <c r="T23" s="49"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="44"/>
+      <c r="P23" s="44"/>
+      <c r="Q23" s="44"/>
+      <c r="R23" s="44"/>
+      <c r="S23" s="44"/>
+      <c r="T23" s="44"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
@@ -3324,25 +3325,25 @@
       <c r="D24" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="E24" s="52">
+      <c r="E24" s="47">
         <v>2</v>
       </c>
-      <c r="F24" s="52">
+      <c r="F24" s="47">
         <v>9</v>
       </c>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="49"/>
-      <c r="O24" s="49"/>
-      <c r="P24" s="49"/>
-      <c r="Q24" s="49"/>
-      <c r="R24" s="49"/>
-      <c r="S24" s="49"/>
-      <c r="T24" s="49"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
+      <c r="P24" s="44"/>
+      <c r="Q24" s="44"/>
+      <c r="R24" s="44"/>
+      <c r="S24" s="44"/>
+      <c r="T24" s="44"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
@@ -3357,25 +3358,25 @@
       <c r="D25" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E25" s="52">
+      <c r="E25" s="47">
         <v>2</v>
       </c>
-      <c r="F25" s="52">
+      <c r="F25" s="47">
         <v>10</v>
       </c>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="49"/>
-      <c r="O25" s="49"/>
-      <c r="P25" s="49"/>
-      <c r="Q25" s="49"/>
-      <c r="R25" s="49"/>
-      <c r="S25" s="49"/>
-      <c r="T25" s="49"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="44"/>
+      <c r="P25" s="44"/>
+      <c r="Q25" s="44"/>
+      <c r="R25" s="44"/>
+      <c r="S25" s="44"/>
+      <c r="T25" s="44"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
@@ -3388,46 +3389,46 @@
         <v>15</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="E26" s="52">
+        <v>135</v>
+      </c>
+      <c r="E26" s="47">
         <v>2</v>
       </c>
-      <c r="F26" s="52">
+      <c r="F26" s="47">
         <v>11</v>
       </c>
-      <c r="H26" s="49"/>
-      <c r="I26" s="49"/>
-      <c r="J26" s="49"/>
-      <c r="K26" s="49"/>
-      <c r="L26" s="49"/>
-      <c r="M26" s="49"/>
-      <c r="N26" s="49"/>
-      <c r="O26" s="49"/>
-      <c r="P26" s="49"/>
-      <c r="Q26" s="49"/>
-      <c r="R26" s="49"/>
-      <c r="S26" s="49"/>
-      <c r="T26" s="49"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
+      <c r="P26" s="44"/>
+      <c r="Q26" s="44"/>
+      <c r="R26" s="44"/>
+      <c r="S26" s="44"/>
+      <c r="T26" s="44"/>
     </row>
     <row r="27" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H27" s="49"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="49"/>
-      <c r="K27" s="49"/>
-      <c r="L27" s="49"/>
-      <c r="M27" s="49"/>
-      <c r="N27" s="49"/>
-      <c r="O27" s="49"/>
-      <c r="P27" s="49"/>
-      <c r="Q27" s="49"/>
-      <c r="R27" s="49"/>
-      <c r="S27" s="49"/>
-      <c r="T27" s="49"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="44"/>
+      <c r="P27" s="44"/>
+      <c r="Q27" s="44"/>
+      <c r="R27" s="44"/>
+      <c r="S27" s="44"/>
+      <c r="T27" s="44"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>12</v>
@@ -3436,42 +3437,42 @@
         <v>16</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E28" s="51">
+        <v>127</v>
+      </c>
+      <c r="E28" s="46">
         <v>2</v>
       </c>
-      <c r="F28" s="51">
+      <c r="F28" s="46">
         <v>13</v>
       </c>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
-      <c r="K28" s="49"/>
-      <c r="L28" s="49"/>
-      <c r="M28" s="49"/>
-      <c r="N28" s="49"/>
-      <c r="O28" s="49"/>
-      <c r="P28" s="49"/>
-      <c r="Q28" s="49"/>
-      <c r="R28" s="49"/>
-      <c r="S28" s="49"/>
-      <c r="T28" s="49"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="44"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="44"/>
+      <c r="O28" s="44"/>
+      <c r="P28" s="44"/>
+      <c r="Q28" s="44"/>
+      <c r="R28" s="44"/>
+      <c r="S28" s="44"/>
+      <c r="T28" s="44"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="H29" s="49"/>
-      <c r="I29" s="49"/>
-      <c r="J29" s="49"/>
-      <c r="K29" s="49"/>
-      <c r="L29" s="49"/>
-      <c r="M29" s="49"/>
-      <c r="N29" s="49"/>
-      <c r="O29" s="49"/>
-      <c r="P29" s="49"/>
-      <c r="Q29" s="49"/>
-      <c r="R29" s="49"/>
-      <c r="S29" s="49"/>
-      <c r="T29" s="49"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="44"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="44"/>
+      <c r="O29" s="44"/>
+      <c r="P29" s="44"/>
+      <c r="Q29" s="44"/>
+      <c r="R29" s="44"/>
+      <c r="S29" s="44"/>
+      <c r="T29" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3487,7 +3488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCAFEBA3-C355-45DA-8226-567ED8EB9D8C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update port planning Documents/Manual_K2_(simple_control_unit).pdf
- VCC encoder from controller now
- KTY room added
- buzzer added
</commit_message>
<xml_diff>
--- a/Documents/Port_Usage_Planning.xlsx
+++ b/Documents/Port_Usage_Planning.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juerg\Documents\_Workspaces\SaunaControlUnit\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7DA0D4-81DE-4035-A1B5-50D86FA12D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E941FA22-BFF3-459E-889C-BA1D0C939ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26850" yWindow="-5150" windowWidth="31100" windowHeight="20460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ESP pin usage" sheetId="6" r:id="rId1"/>
-    <sheet name="All signals" sheetId="1" r:id="rId2"/>
+    <sheet name="Signal view" sheetId="1" r:id="rId1"/>
+    <sheet name="ESP module view" sheetId="6" r:id="rId2"/>
     <sheet name="ESP32-Pinout" sheetId="2" r:id="rId3"/>
-    <sheet name="Schematic" sheetId="5" r:id="rId4"/>
-    <sheet name="KTY" sheetId="4" r:id="rId5"/>
-    <sheet name="LCD SPI" sheetId="3" r:id="rId6"/>
+    <sheet name="Schematic ESP" sheetId="5" r:id="rId4"/>
+    <sheet name="Schematic LCD SPI" sheetId="3" r:id="rId5"/>
+    <sheet name="KTY" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="150">
   <si>
     <t>Funktion</t>
   </si>
@@ -406,9 +406,6 @@
     <t>ENC_CLK</t>
   </si>
   <si>
-    <t>ESP32 necessary signals</t>
-  </si>
-  <si>
     <t>Stift
 reihe</t>
   </si>
@@ -437,18 +434,63 @@
     <t>Digital PWM-Output</t>
   </si>
   <si>
-    <t>The pins D0, D1, D2, D3, CMD and CLK are used internally for communication between ESP32 and SPI flash memory. 
-They are grouped on both sides near the USB connector. Avoid using these pins, as it may disrupt access to the SPI flash memory/SPI RAM.</t>
-  </si>
-  <si>
     <t>GPIO17</t>
+  </si>
+  <si>
+    <t>ENC_VCC</t>
+  </si>
+  <si>
+    <t>GPIO16</t>
+  </si>
+  <si>
+    <t>reserved</t>
+  </si>
+  <si>
+    <t>Pwr</t>
+  </si>
+  <si>
+    <t>Buzzer</t>
+  </si>
+  <si>
+    <t>KTY room input</t>
+  </si>
+  <si>
+    <t>KTY oven input</t>
+  </si>
+  <si>
+    <t>ADC2_CH1</t>
+  </si>
+  <si>
+    <t>GPIO2</t>
+  </si>
+  <si>
+    <t>N.A.</t>
+  </si>
+  <si>
+    <t>Internally used for communication ESP and flash memory.
+Do not use!</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Chip function</t>
+  </si>
+  <si>
+    <t>Signal view</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>ESP module connector view</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -480,8 +522,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -518,8 +568,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -680,13 +736,125 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -837,29 +1005,85 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Überschrift 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -990,6 +1214,55 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>260351</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>673101</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>108947</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8EEFCDC-A296-9AAE-7007-200C107F11A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="260351" y="0"/>
+          <a:ext cx="16414750" cy="9824447"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1388,837 +1661,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9221DBC-EDCA-460E-9237-EA76481AB5F0}">
-  <dimension ref="A1:M29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:M25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="3" width="6.6328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.08984375" customWidth="1"/>
-    <col min="6" max="6" width="39.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.54296875" customWidth="1"/>
-    <col min="8" max="10" width="6.6328125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.54296875" customWidth="1"/>
-    <col min="12" max="12" width="14.26953125" customWidth="1"/>
-    <col min="13" max="13" width="34.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="59" t="s">
-        <v>129</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="H1" s="59" t="s">
-        <v>130</v>
-      </c>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="21">
-        <v>1</v>
-      </c>
-      <c r="B3" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="21">
-        <v>1</v>
-      </c>
-      <c r="I3" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="21">
-        <v>2</v>
-      </c>
-      <c r="B4" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="21">
-        <v>2</v>
-      </c>
-      <c r="I4" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="J4" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="23">
-        <v>3</v>
-      </c>
-      <c r="B5" s="54" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="54" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="34">
-        <v>3</v>
-      </c>
-      <c r="I5" s="52" t="s">
-        <v>64</v>
-      </c>
-      <c r="J5" s="52" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="M5" s="35" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="23">
-        <v>4</v>
-      </c>
-      <c r="B6" s="54" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="54" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="21">
-        <v>4</v>
-      </c>
-      <c r="I6" s="51" t="s">
-        <v>66</v>
-      </c>
-      <c r="J6" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="22" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="23">
-        <v>5</v>
-      </c>
-      <c r="B7" s="54" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="54" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="21">
-        <v>5</v>
-      </c>
-      <c r="I7" s="51" t="s">
-        <v>68</v>
-      </c>
-      <c r="J7" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="23">
-        <v>6</v>
-      </c>
-      <c r="B8" s="54" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="54" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="34">
-        <v>6</v>
-      </c>
-      <c r="I8" s="52" t="s">
-        <v>70</v>
-      </c>
-      <c r="J8" s="52" t="s">
-        <v>35</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="M8" s="35" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="25">
-        <v>7</v>
-      </c>
-      <c r="B9" s="57" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="21">
-        <v>7</v>
-      </c>
-      <c r="I9" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="J9" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="25">
-        <v>8</v>
-      </c>
-      <c r="B10" s="57" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="27">
-        <v>8</v>
-      </c>
-      <c r="I10" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="J10" s="53" t="s">
-        <v>35</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="M10" s="28" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="25">
-        <v>9</v>
-      </c>
-      <c r="B11" s="57" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="43">
-        <v>9</v>
-      </c>
-      <c r="I11" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="J11" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="M11" s="29" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="27">
-        <v>10</v>
-      </c>
-      <c r="B12" s="53" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="53" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="H12" s="43">
-        <v>10</v>
-      </c>
-      <c r="I12" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="J12" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="L12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="M12" s="29" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="27">
-        <v>11</v>
-      </c>
-      <c r="B13" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="53" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="F13" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="H13" s="43">
-        <v>11</v>
-      </c>
-      <c r="I13" s="47" t="s">
-        <v>77</v>
-      </c>
-      <c r="J13" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="L13" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="M13" s="29" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="27">
-        <v>12</v>
-      </c>
-      <c r="B14" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="53" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="F14" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="H14" s="21">
-        <v>12</v>
-      </c>
-      <c r="I14" s="51" t="s">
-        <v>79</v>
-      </c>
-      <c r="J14" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="30" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="25">
-        <v>13</v>
-      </c>
-      <c r="B15" s="57" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="H15" s="23">
-        <v>13</v>
-      </c>
-      <c r="I15" s="54" t="s">
-        <v>81</v>
-      </c>
-      <c r="J15" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="M15" s="24" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="21">
-        <v>14</v>
-      </c>
-      <c r="B16" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="H16" s="21">
-        <v>14</v>
-      </c>
-      <c r="I16" s="51" t="s">
-        <v>83</v>
-      </c>
-      <c r="J16" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="25">
-        <v>15</v>
-      </c>
-      <c r="B17" s="57" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="21">
-        <v>16</v>
-      </c>
-      <c r="I17" s="51" t="s">
-        <v>85</v>
-      </c>
-      <c r="J17" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="22" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="36">
-        <v>16</v>
-      </c>
-      <c r="B18" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="H18" s="43">
-        <v>17</v>
-      </c>
-      <c r="I18" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="J18" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="L18" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="M18" s="29" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="36">
-        <v>17</v>
-      </c>
-      <c r="B19" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="H19" s="36">
-        <v>17</v>
-      </c>
-      <c r="I19" s="55" t="s">
-        <v>89</v>
-      </c>
-      <c r="J19" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="38" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="36">
-        <v>18</v>
-      </c>
-      <c r="B20" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="H20" s="36">
-        <v>18</v>
-      </c>
-      <c r="I20" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="J20" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="K20" s="37"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="38" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="31">
-        <v>19</v>
-      </c>
-      <c r="B21" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="58" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="H21" s="40">
-        <v>19</v>
-      </c>
-      <c r="I21" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="J21" s="56" t="s">
-        <v>35</v>
-      </c>
-      <c r="K21" s="41"/>
-      <c r="L21" s="41"/>
-      <c r="M21" s="42" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="61" t="s">
-        <v>116</v>
-      </c>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="60"/>
-      <c r="M23" s="60"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" s="4"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="61" t="s">
-        <v>117</v>
-      </c>
-      <c r="B25" s="60"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="60"/>
-      <c r="I25" s="60"/>
-      <c r="J25" s="60"/>
-      <c r="K25" s="60"/>
-      <c r="L25" s="60"/>
-      <c r="M25" s="60"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="4"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="62" t="s">
-        <v>134</v>
-      </c>
-      <c r="B27" s="62"/>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="62"/>
-      <c r="K27" s="62"/>
-      <c r="L27" s="62"/>
-      <c r="M27" s="62"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="62"/>
-      <c r="B28" s="62"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="62"/>
-      <c r="H28" s="62"/>
-      <c r="I28" s="62"/>
-      <c r="J28" s="62"/>
-      <c r="K28" s="62"/>
-      <c r="L28" s="62"/>
-      <c r="M28" s="62"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="62"/>
-      <c r="B29" s="62"/>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="62"/>
-      <c r="G29" s="62"/>
-      <c r="H29" s="62"/>
-      <c r="I29" s="62"/>
-      <c r="J29" s="62"/>
-      <c r="K29" s="62"/>
-      <c r="L29" s="62"/>
-      <c r="M29" s="62"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="A23:M23"/>
-    <mergeCell ref="A25:M25"/>
-    <mergeCell ref="A27:M29"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A25" r:id="rId1" xr:uid="{8C29EB1E-5FC7-4B4B-B6D2-9EF086296AB7}"/>
-    <hyperlink ref="A23" r:id="rId2" xr:uid="{66CDB618-6607-4CC0-9408-30BF1EA62DE2}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T29"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2244,31 +1691,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="63" t="s">
-        <v>124</v>
-      </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
+      <c r="A1" s="66" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="59" t="s">
+      <c r="H1" s="68" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="O1" s="68" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="O1" s="59" t="s">
-        <v>130</v>
-      </c>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="68"/>
+      <c r="T1" s="68"/>
     </row>
     <row r="2" spans="1:20" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
@@ -2284,7 +1731,7 @@
         <v>99</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F2" s="45" t="s">
         <v>100</v>
@@ -2302,7 +1749,7 @@
         <v>4</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M2" s="20" t="s">
         <v>19</v>
@@ -2761,7 +2208,7 @@
         <v>35</v>
       </c>
       <c r="R11" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S11" s="9" t="s">
         <v>13</v>
@@ -2975,7 +2422,7 @@
         <v>35</v>
       </c>
       <c r="R15" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S15" s="7" t="s">
         <v>12</v>
@@ -3097,7 +2544,7 @@
         <v>15</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E18" s="47">
         <v>2</v>
@@ -3289,6 +2736,9 @@
       </c>
       <c r="F22" s="49">
         <v>8</v>
+      </c>
+      <c r="N22" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.35">
@@ -3389,7 +2839,7 @@
         <v>15</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E26" s="47">
         <v>2</v>
@@ -3411,7 +2861,25 @@
       <c r="S26" s="44"/>
       <c r="T26" s="44"/>
     </row>
-    <row r="27" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A27" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27" s="49">
+        <v>2</v>
+      </c>
+      <c r="F27" s="49">
+        <v>12</v>
+      </c>
       <c r="H27" s="44"/>
       <c r="I27" s="44"/>
       <c r="J27" s="44"/>
@@ -3427,23 +2895,23 @@
       <c r="T27" s="44"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A28" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="E28" s="46">
+      <c r="A28" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="E28" s="49">
         <v>2</v>
       </c>
-      <c r="F28" s="46">
-        <v>13</v>
+      <c r="F28" s="49">
+        <v>24</v>
       </c>
       <c r="H28" s="44"/>
       <c r="I28" s="44"/>
@@ -3459,7 +2927,7 @@
       <c r="S28" s="44"/>
       <c r="T28" s="44"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H29" s="44"/>
       <c r="I29" s="44"/>
       <c r="J29" s="44"/>
@@ -3474,6 +2942,87 @@
       <c r="S29" s="44"/>
       <c r="T29" s="44"/>
     </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30" s="46">
+        <v>2</v>
+      </c>
+      <c r="F30" s="46">
+        <v>13</v>
+      </c>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="44"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="44"/>
+      <c r="O30" s="44"/>
+      <c r="P30" s="44"/>
+      <c r="Q30" s="44"/>
+      <c r="R30" s="44"/>
+      <c r="S30" s="44"/>
+      <c r="T30" s="44"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A31" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E31" s="46">
+        <v>2</v>
+      </c>
+      <c r="F31" s="46">
+        <v>14</v>
+      </c>
+      <c r="H31" s="44"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="44"/>
+      <c r="L31" s="44"/>
+      <c r="M31" s="44"/>
+      <c r="N31" s="44"/>
+      <c r="O31" s="44"/>
+      <c r="P31" s="44"/>
+      <c r="Q31" s="44"/>
+      <c r="R31" s="44"/>
+      <c r="S31" s="44"/>
+      <c r="T31" s="44"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="H32" s="44"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="44"/>
+      <c r="L32" s="44"/>
+      <c r="M32" s="44"/>
+      <c r="N32" s="44"/>
+      <c r="O32" s="44"/>
+      <c r="P32" s="44"/>
+      <c r="Q32" s="44"/>
+      <c r="R32" s="44"/>
+      <c r="S32" s="44"/>
+      <c r="T32" s="44"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="H1:M1"/>
@@ -3481,6 +3030,831 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9221DBC-EDCA-460E-9237-EA76481AB5F0}">
+  <dimension ref="A1:M26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="6.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.08984375" customWidth="1"/>
+    <col min="6" max="6" width="39.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.54296875" customWidth="1"/>
+    <col min="8" max="10" width="6.6328125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.54296875" customWidth="1"/>
+    <col min="12" max="12" width="14.26953125" customWidth="1"/>
+    <col min="13" max="13" width="34.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="66" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+    </row>
+    <row r="2" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="H3" s="68" t="s">
+        <v>129</v>
+      </c>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+    </row>
+    <row r="4" spans="1:13" s="65" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="63" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" s="64" t="s">
+        <v>146</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="K4" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="63" t="s">
+        <v>145</v>
+      </c>
+      <c r="M4" s="64" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="59">
+        <v>1</v>
+      </c>
+      <c r="B5" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="59">
+        <v>1</v>
+      </c>
+      <c r="I5" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="K5" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="L5" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="M5" s="62" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="21">
+        <v>2</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="21">
+        <v>2</v>
+      </c>
+      <c r="I6" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="23">
+        <v>3</v>
+      </c>
+      <c r="B7" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="34">
+        <v>3</v>
+      </c>
+      <c r="I7" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="M7" s="35" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="23">
+        <v>4</v>
+      </c>
+      <c r="B8" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="21">
+        <v>4</v>
+      </c>
+      <c r="I8" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="23">
+        <v>5</v>
+      </c>
+      <c r="B9" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="21">
+        <v>5</v>
+      </c>
+      <c r="I9" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="23">
+        <v>6</v>
+      </c>
+      <c r="B10" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="34">
+        <v>6</v>
+      </c>
+      <c r="I10" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="M10" s="35" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="25">
+        <v>7</v>
+      </c>
+      <c r="B11" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="59">
+        <v>7</v>
+      </c>
+      <c r="I11" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="K11" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="L11" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="M11" s="62" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="25">
+        <v>8</v>
+      </c>
+      <c r="B12" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" s="27">
+        <v>8</v>
+      </c>
+      <c r="I12" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" s="28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" s="25">
+        <v>9</v>
+      </c>
+      <c r="B13" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="43">
+        <v>9</v>
+      </c>
+      <c r="I13" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="J13" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M13" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="27">
+        <v>10</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" s="43">
+        <v>10</v>
+      </c>
+      <c r="I14" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="J14" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="27">
+        <v>11</v>
+      </c>
+      <c r="B15" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="43">
+        <v>11</v>
+      </c>
+      <c r="I15" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="J15" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M15" s="29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" s="27">
+        <v>12</v>
+      </c>
+      <c r="B16" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="27">
+        <v>12</v>
+      </c>
+      <c r="I16" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="J16" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16" s="28" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" s="25">
+        <v>13</v>
+      </c>
+      <c r="B17" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="23">
+        <v>13</v>
+      </c>
+      <c r="I17" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="J17" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M17" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="59">
+        <v>14</v>
+      </c>
+      <c r="B18" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="D18" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="E18" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="F18" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="23">
+        <v>14</v>
+      </c>
+      <c r="I18" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="J18" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M18" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" s="25">
+        <v>15</v>
+      </c>
+      <c r="B19" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="27">
+        <v>16</v>
+      </c>
+      <c r="I19" s="53" t="s">
+        <v>85</v>
+      </c>
+      <c r="J19" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="L19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="M19" s="28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="36">
+        <v>16</v>
+      </c>
+      <c r="B20" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="71" t="s">
+        <v>144</v>
+      </c>
+      <c r="E20" s="72"/>
+      <c r="F20" s="73"/>
+      <c r="H20" s="43">
+        <v>17</v>
+      </c>
+      <c r="I20" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="J20" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M20" s="29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" s="36">
+        <v>17</v>
+      </c>
+      <c r="B21" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="74"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="76"/>
+      <c r="H21" s="36">
+        <v>17</v>
+      </c>
+      <c r="I21" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="J21" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="K21" s="71" t="s">
+        <v>144</v>
+      </c>
+      <c r="L21" s="72"/>
+      <c r="M21" s="73"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" s="36">
+        <v>18</v>
+      </c>
+      <c r="B22" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="77"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="79"/>
+      <c r="H22" s="36">
+        <v>18</v>
+      </c>
+      <c r="I22" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="J22" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="K22" s="74"/>
+      <c r="L22" s="75"/>
+      <c r="M22" s="76"/>
+    </row>
+    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="59">
+        <v>19</v>
+      </c>
+      <c r="B23" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="E23" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="F23" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" s="40">
+        <v>19</v>
+      </c>
+      <c r="I23" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="J23" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="K23" s="80"/>
+      <c r="L23" s="81"/>
+      <c r="M23" s="82"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" s="69" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" s="70"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="70"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="70"/>
+      <c r="J25" s="70"/>
+      <c r="K25" s="70"/>
+      <c r="L25" s="70"/>
+      <c r="M25" s="70"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" s="69" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="70"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="70"/>
+      <c r="J26" s="70"/>
+      <c r="K26" s="70"/>
+      <c r="L26" s="70"/>
+      <c r="M26" s="70"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="A25:M25"/>
+    <mergeCell ref="A26:M26"/>
+    <mergeCell ref="D20:F22"/>
+    <mergeCell ref="K21:M23"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A26" r:id="rId1" xr:uid="{8C29EB1E-5FC7-4B4B-B6D2-9EF086296AB7}"/>
+    <hyperlink ref="A25" r:id="rId2" xr:uid="{66CDB618-6607-4CC0-9408-30BF1EA62DE2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3519,6 +3893,27 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA904A2-683C-4976-B307-148881F494F2}">
+  <dimension ref="Q22"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="22" spans="17:17" x14ac:dyDescent="0.35">
+      <c r="Q22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE5AC62-314B-48A8-8608-6F7F7B159042}">
   <dimension ref="A26"/>
   <sheetViews>
@@ -3537,18 +3932,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA904A2-683C-4976-B307-148881F494F2}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Backlight signal removed two debug pins added remarks regarding KTY added
</commit_message>
<xml_diff>
--- a/Documents/Port_Usage_Planning.xlsx
+++ b/Documents/Port_Usage_Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juerg\Documents\_Workspaces\SaunaControlUnit\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bekone01-my.sharepoint.com/personal/juergen_eggeling_beko-technologies_com/Documents/_Projekte/_Bastelprojekte/SaunaControlUnit/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E941FA22-BFF3-459E-889C-BA1D0C939ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{E941FA22-BFF3-459E-889C-BA1D0C939ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A52A154C-65FC-471F-A41E-ED115C467187}"/>
   <bookViews>
-    <workbookView xWindow="26850" yWindow="-5150" windowWidth="31100" windowHeight="20460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32220" yWindow="3420" windowWidth="38700" windowHeight="15225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Signal view" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="152">
   <si>
     <t>Funktion</t>
   </si>
@@ -484,6 +484,12 @@
   </si>
   <si>
     <t>ESP module connector view</t>
+  </si>
+  <si>
+    <t>Debug_1</t>
+  </si>
+  <si>
+    <t>Debug_2</t>
   </si>
 </sst>
 </file>
@@ -1027,13 +1033,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -1691,31 +1697,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="67" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="68" t="s">
+      <c r="H1" s="66" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="O1" s="68" t="s">
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="O1" s="66" t="s">
         <v>129</v>
       </c>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
     </row>
     <row r="2" spans="1:20" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
@@ -3038,7 +3044,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3055,40 +3061,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="67" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
     </row>
     <row r="2" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="68" t="s">
         <v>128</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="H3" s="68" t="s">
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="H3" s="66" t="s">
         <v>129</v>
       </c>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="68"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="66"/>
     </row>
     <row r="4" spans="1:13" s="65" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
@@ -3185,18 +3191,22 @@
       <c r="F6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6" s="27">
         <v>2</v>
       </c>
-      <c r="I6" s="51" t="s">
+      <c r="I6" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="J6" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="22" t="s">
+      <c r="J6" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="28" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3411,7 +3421,7 @@
         <v>35</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>118</v>
+        <v>150</v>
       </c>
       <c r="L12" s="11" t="s">
         <v>14</v>

</xml_diff>